<commit_message>
Updated Documentation and Source
</commit_message>
<xml_diff>
--- a/docs/Device Opcodes.xlsx
+++ b/docs/Device Opcodes.xlsx
@@ -271,9 +271,6 @@
     <t>0x57</t>
   </si>
   <si>
-    <t>Phoenix</t>
-  </si>
-  <si>
     <t>Supported Commands</t>
   </si>
   <si>
@@ -286,117 +283,6 @@
     <t>AT25SF041</t>
   </si>
   <si>
-    <t>CMD_PHOENIX_READ_ARRAY_HF</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_READ_ARRAY_LF</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_DUAL_OUTPUT_READ</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_DUAL_IO_READ</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_QUAD_OUTPUT_READ</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_QUAD_IO_READ</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_CONT_READ_MODE_RST_DUAL</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_CONT_READ_MODE_RST_QUAD</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_BLOCK_ERASE_4K</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_BLOCK_ERASE_32K</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_BLOCK_ERASE_64K</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_CHIP_ERASE1</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_CHIP_ERASE2</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_BYTE_PAGE_PROGRAM</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_WRITE_ENABLE</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_WRITE_DISABLE</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_ERASE_SECURTIY_REG_PAGE</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_PROGRAM_SECURITY_REG_PAGE</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_READ_SECURITY_REG_PAGE</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_READ_SRB1</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_READ_SRB2</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_WRITE_SR</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_WE_FOR_VOLATILE_SR</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_READ_MID</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_READ_ID</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_DEEP_POWER_DOWN</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_RESUME_FROM_DPD</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_RESUME_FROM_DPD_READ_ID</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_QUAD_PAGE_PROGRAM</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_ENABLE_QPI</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_DISABLE_QPI</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_ERASE_PROGRAM_SUSPEND</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_ERASE_PROGRAM_RESUME</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_ENABLE_RESET</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_RESET</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_ENTER_SECURED_OTP</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_EXIT_SECURED_OTP</t>
-  </si>
-  <si>
     <t>Command Name</t>
   </si>
   <si>
@@ -889,19 +775,133 @@
     <t>CMD_DATAFLASH_QUAD_DISABLE</t>
   </si>
   <si>
-    <t>CMD_PHOENIX_READ_SR</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_WRITE_SRB1</t>
-  </si>
-  <si>
-    <t>CMD_PHOENIX_WRITE_SRB2</t>
-  </si>
-  <si>
     <t>2 bytes possible</t>
   </si>
   <si>
     <t>1 byte only</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASAH_DUAL_OUTPUT_READ</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASAH_DUAL_IO_READ</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASAH_QUAD_OUTPUT_READ</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASAH_QUAD_IO_READ</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASAH_QUAD_PAGE_PROGRAM</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASAH_CONT_READ_MODE_RST_DUAL</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASAH_CONT_READ_MODE_RST_QUAD</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASAH_ERASE_SECURTIY_REG_PAGE</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASAH_PROGRAM_SECURITY_REG_PAGE</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASAH_READ_SECURITY_REG_PAGE</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASAH_RESUME_FROM_DPD_READ_ID</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASAH_DISABLE_QPI</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_WRITE_ENABLE</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_WE_FOR_VOLATILE_SR</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_WRITE_DISABLE</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_READ_SR</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_READ_SRB1</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_READ_SRB2</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_WRITE_SR</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_WRITE_SRB1</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_WRITE_SRB2</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_READ_ARRAY_LF</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_READ_ARRAY_HF</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_BYTE_PAGE_PROGRAM</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_ENABLE_QPI</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_BLOCK_ERASE_4K</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_BLOCK_ERASE_32K</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_BLOCK_ERASE_64K</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_CHIP_ERASE1</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_CHIP_ERASE2</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_ERASE_PROGRAM_SUSPEND</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_ERASE_PROGRAM_RESUME</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_DEEP_POWER_DOWN</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_RESUME_FROM_DPD</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_READ_ID</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_READ_MID</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_ENABLE_RESET</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_RESET</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_ENTER_SECURED_OTP</t>
+  </si>
+  <si>
+    <t>CMD_STANDARDFLASH_EXIT_SECURED_OTP</t>
+  </si>
+  <si>
+    <t>Standardflash</t>
   </si>
 </sst>
 </file>
@@ -1326,8 +1326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U178"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1354,12 +1354,12 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>85</v>
+        <v>295</v>
       </c>
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
@@ -1369,63 +1369,63 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>263</v>
+        <v>225</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>262</v>
+        <v>224</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>261</v>
+        <v>223</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
       <c r="N4" s="9" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
       <c r="O4" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
       <c r="P4" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="Q4" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>272</v>
+        <v>234</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>267</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -1481,7 +1481,7 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>112</v>
+        <v>268</v>
       </c>
       <c r="B6" t="s">
         <v>22</v>
@@ -1522,7 +1522,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>269</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
@@ -1578,7 +1578,7 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
       <c r="J8" t="s">
         <v>19</v>
@@ -1598,7 +1598,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>271</v>
       </c>
       <c r="B9" t="s">
         <v>19</v>
@@ -1639,7 +1639,7 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>272</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
@@ -1680,7 +1680,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>111</v>
+        <v>273</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
@@ -1697,7 +1697,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>292</v>
+        <v>274</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>21</v>
@@ -1739,15 +1739,15 @@
         <v>21</v>
       </c>
       <c r="T12" s="10" t="s">
-        <v>294</v>
+        <v>253</v>
       </c>
       <c r="U12" s="11" t="s">
-        <v>295</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="F13" t="s">
         <v>35</v>
@@ -1791,7 +1791,7 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>276</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
@@ -1847,7 +1847,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>277</v>
       </c>
       <c r="B15" t="s">
         <v>0</v>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>278</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
@@ -1959,7 +1959,7 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>279</v>
       </c>
       <c r="F17" t="s">
         <v>28</v>
@@ -1988,7 +1988,7 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>98</v>
+        <v>280</v>
       </c>
       <c r="B18" t="s">
         <v>8</v>
@@ -2044,7 +2044,7 @@
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>99</v>
+        <v>281</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
@@ -2100,7 +2100,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>100</v>
+        <v>282</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -2156,7 +2156,7 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>283</v>
       </c>
       <c r="B21" t="s">
         <v>11</v>
@@ -2212,7 +2212,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>284</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
@@ -2268,7 +2268,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>285</v>
       </c>
       <c r="D23" t="s">
         <v>29</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>286</v>
       </c>
       <c r="D24" t="s">
         <v>30</v>
@@ -2338,7 +2338,7 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>115</v>
+        <v>287</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
@@ -2394,7 +2394,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>116</v>
+        <v>288</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
@@ -2450,7 +2450,7 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>114</v>
+        <v>289</v>
       </c>
       <c r="B27" t="s">
         <v>24</v>
@@ -2491,7 +2491,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>113</v>
+        <v>290</v>
       </c>
       <c r="B28" t="s">
         <v>23</v>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>123</v>
+        <v>291</v>
       </c>
       <c r="F29" t="s">
         <v>31</v>
@@ -2576,7 +2576,7 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>124</v>
+        <v>292</v>
       </c>
       <c r="F30" t="s">
         <v>32</v>
@@ -2605,7 +2605,7 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>125</v>
+        <v>293</v>
       </c>
       <c r="F31" t="s">
         <v>33</v>
@@ -2634,7 +2634,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>126</v>
+        <v>294</v>
       </c>
       <c r="F32" t="s">
         <v>34</v>
@@ -2663,85 +2663,85 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F33" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="G33" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="H33" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="I33" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="O33" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="P33" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="Q33" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
       <c r="R33" t="s">
-        <v>273</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F34" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="G34" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="H34" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="I34" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="O34" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="P34" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="Q34" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
       <c r="R34" t="s">
-        <v>274</v>
+        <v>236</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F35" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="G35" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="H35" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="I35" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="O35" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="P35" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="Q35" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
       <c r="R35" t="s">
-        <v>275</v>
+        <v>237</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>92</v>
+        <v>255</v>
       </c>
       <c r="B36" t="s">
         <v>2</v>
@@ -2782,7 +2782,7 @@
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>93</v>
+        <v>256</v>
       </c>
       <c r="B37" t="s">
         <v>3</v>
@@ -2823,33 +2823,33 @@
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F38" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="G38" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="H38" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="I38" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="O38" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="P38" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="Q38" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
       <c r="R38" t="s">
-        <v>276</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>94</v>
+        <v>257</v>
       </c>
       <c r="B39" t="s">
         <v>4</v>
@@ -2890,7 +2890,7 @@
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>95</v>
+        <v>258</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
@@ -2931,7 +2931,7 @@
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>259</v>
       </c>
       <c r="F41" t="s">
         <v>27</v>
@@ -2975,54 +2975,54 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F42" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
       <c r="G42" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
       <c r="H42" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
       <c r="I42" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
       <c r="O42" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
       <c r="P42" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
       <c r="Q42" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
       <c r="R42" t="s">
-        <v>277</v>
+        <v>239</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="F43" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="G43" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="H43" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="I43" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="O43" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="P43" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="Q43" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
       <c r="R43" t="s">
-        <v>278</v>
+        <v>240</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
@@ -3068,7 +3068,7 @@
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>96</v>
+        <v>260</v>
       </c>
       <c r="B45" t="s">
         <v>6</v>
@@ -3109,7 +3109,7 @@
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>261</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
@@ -3150,7 +3150,7 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>106</v>
+        <v>262</v>
       </c>
       <c r="B47" t="s">
         <v>16</v>
@@ -3191,7 +3191,7 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>263</v>
       </c>
       <c r="B48" t="s">
         <v>17</v>
@@ -3232,7 +3232,7 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>108</v>
+        <v>264</v>
       </c>
       <c r="B49" t="s">
         <v>18</v>
@@ -3273,7 +3273,7 @@
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>117</v>
+        <v>265</v>
       </c>
       <c r="B50" t="s">
         <v>26</v>
@@ -3314,7 +3314,7 @@
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>120</v>
+        <v>266</v>
       </c>
       <c r="F51" t="s">
         <v>7</v>
@@ -3439,19 +3439,19 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J58" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
       <c r="K58" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
       <c r="L58" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
       <c r="M58" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
       <c r="N58" t="s">
-        <v>279</v>
+        <v>241</v>
       </c>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
@@ -3473,58 +3473,58 @@
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="J60" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="K60" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="L60" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="M60" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="N60" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="B64" t="s">
-        <v>222</v>
+        <v>184</v>
       </c>
       <c r="C64" t="s">
-        <v>223</v>
+        <v>185</v>
       </c>
       <c r="D64" t="s">
-        <v>224</v>
+        <v>186</v>
       </c>
       <c r="E64" t="s">
-        <v>131</v>
+        <v>93</v>
       </c>
       <c r="F64" t="s">
-        <v>280</v>
+        <v>242</v>
       </c>
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>132</v>
+        <v>94</v>
       </c>
       <c r="B65" t="s">
-        <v>225</v>
+        <v>187</v>
       </c>
       <c r="C65" t="s">
-        <v>225</v>
+        <v>187</v>
       </c>
       <c r="D65" t="s">
-        <v>225</v>
+        <v>187</v>
       </c>
       <c r="F65" t="s">
         <v>14</v>
@@ -3532,7 +3532,7 @@
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>133</v>
+        <v>95</v>
       </c>
       <c r="F66" t="s">
         <v>15</v>
@@ -3540,7 +3540,7 @@
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="F67" t="s">
         <v>19</v>
@@ -3548,7 +3548,7 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>135</v>
+        <v>97</v>
       </c>
       <c r="F68" t="s">
         <v>21</v>
@@ -3556,7 +3556,7 @@
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="F69" t="s">
         <v>35</v>
@@ -3564,7 +3564,7 @@
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>137</v>
+        <v>99</v>
       </c>
       <c r="F70" t="s">
         <v>1</v>
@@ -3572,7 +3572,7 @@
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>138</v>
+        <v>100</v>
       </c>
       <c r="F71" t="s">
         <v>13</v>
@@ -3580,7 +3580,7 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>139</v>
+        <v>101</v>
       </c>
       <c r="F72" t="s">
         <v>23</v>
@@ -3588,7 +3588,7 @@
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>140</v>
+        <v>102</v>
       </c>
       <c r="F73" t="s">
         <v>36</v>
@@ -3596,12 +3596,12 @@
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F74" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="F75" t="s">
-        <v>281</v>
+        <v>243</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.25">
@@ -3611,59 +3611,59 @@
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>141</v>
+        <v>103</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>230</v>
+        <v>192</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>231</v>
+        <v>193</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>232</v>
+        <v>194</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>229</v>
+        <v>191</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>251</v>
+        <v>213</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>253</v>
+        <v>215</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>255</v>
+        <v>217</v>
       </c>
       <c r="I80" s="6" t="s">
-        <v>252</v>
+        <v>214</v>
       </c>
       <c r="J80" s="6" t="s">
-        <v>254</v>
+        <v>216</v>
       </c>
       <c r="K80" s="6" t="s">
-        <v>256</v>
+        <v>218</v>
       </c>
       <c r="L80" s="6" t="s">
-        <v>257</v>
+        <v>219</v>
       </c>
       <c r="M80" s="6" t="s">
-        <v>258</v>
+        <v>220</v>
       </c>
       <c r="N80" s="4" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="O80" s="4" t="s">
-        <v>260</v>
+        <v>222</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>149</v>
+        <v>111</v>
       </c>
       <c r="B81" t="s">
         <v>0</v>
@@ -3710,7 +3710,7 @@
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="B82" t="s">
         <v>1</v>
@@ -3757,7 +3757,7 @@
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>158</v>
+        <v>120</v>
       </c>
       <c r="B83" t="s">
         <v>2</v>
@@ -3804,7 +3804,7 @@
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>150</v>
+        <v>112</v>
       </c>
       <c r="B84" t="s">
         <v>40</v>
@@ -3851,7 +3851,7 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>151</v>
+        <v>113</v>
       </c>
       <c r="B85" t="s">
         <v>8</v>
@@ -3986,7 +3986,7 @@
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>152</v>
+        <v>114</v>
       </c>
       <c r="B88" t="s">
         <v>11</v>
@@ -4077,7 +4077,7 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>154</v>
+        <v>116</v>
       </c>
       <c r="B90" t="s">
         <v>13</v>
@@ -4124,7 +4124,7 @@
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>157</v>
+        <v>119</v>
       </c>
       <c r="D91" t="s">
         <v>41</v>
@@ -4147,27 +4147,27 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D92" t="s">
-        <v>226</v>
+        <v>188</v>
       </c>
       <c r="E92" t="s">
-        <v>226</v>
+        <v>188</v>
       </c>
       <c r="L92" t="s">
-        <v>226</v>
+        <v>188</v>
       </c>
       <c r="M92" t="s">
-        <v>226</v>
+        <v>188</v>
       </c>
       <c r="N92" t="s">
-        <v>226</v>
+        <v>188</v>
       </c>
       <c r="O92" t="s">
-        <v>226</v>
+        <v>188</v>
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>159</v>
+        <v>121</v>
       </c>
       <c r="D93" t="s">
         <v>42</v>
@@ -4190,7 +4190,7 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="B94" t="s">
         <v>14</v>
@@ -4237,7 +4237,7 @@
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="B95" t="s">
         <v>15</v>
@@ -4284,7 +4284,7 @@
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>145</v>
+        <v>107</v>
       </c>
       <c r="D96" t="s">
         <v>38</v>
@@ -4307,7 +4307,7 @@
     </row>
     <row r="97" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>144</v>
+        <v>106</v>
       </c>
       <c r="D97" t="s">
         <v>37</v>
@@ -4330,7 +4330,7 @@
     </row>
     <row r="98" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
       <c r="D98" t="s">
         <v>39</v>
@@ -4353,46 +4353,46 @@
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="C99" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="D99" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="E99" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="F99" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="G99" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="H99" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="I99" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="J99" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="K99" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="L99" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="M99" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="N99" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
       <c r="O99" t="s">
-        <v>227</v>
+        <v>189</v>
       </c>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.25">
@@ -4441,7 +4441,7 @@
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>153</v>
+        <v>115</v>
       </c>
       <c r="B101" t="s">
         <v>19</v>
@@ -4488,27 +4488,27 @@
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D102" t="s">
-        <v>228</v>
+        <v>190</v>
       </c>
       <c r="E102" t="s">
-        <v>228</v>
+        <v>190</v>
       </c>
       <c r="L102" t="s">
-        <v>228</v>
+        <v>190</v>
       </c>
       <c r="M102" t="s">
-        <v>228</v>
+        <v>190</v>
       </c>
       <c r="N102" t="s">
-        <v>228</v>
+        <v>190</v>
       </c>
       <c r="O102" t="s">
-        <v>228</v>
+        <v>190</v>
       </c>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>155</v>
+        <v>117</v>
       </c>
       <c r="B103" t="s">
         <v>21</v>
@@ -4555,7 +4555,7 @@
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>156</v>
+        <v>118</v>
       </c>
       <c r="B104" t="s">
         <v>35</v>
@@ -4602,7 +4602,7 @@
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
       <c r="B105" t="s">
         <v>43</v>
@@ -4649,7 +4649,7 @@
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="B106" t="s">
         <v>23</v>
@@ -4696,7 +4696,7 @@
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>160</v>
+        <v>122</v>
       </c>
       <c r="B107" t="s">
         <v>25</v>
@@ -4743,7 +4743,7 @@
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>161</v>
+        <v>123</v>
       </c>
       <c r="B108" t="s">
         <v>26</v>
@@ -4790,7 +4790,7 @@
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>163</v>
+        <v>125</v>
       </c>
       <c r="B109" t="s">
         <v>36</v>
@@ -4837,53 +4837,53 @@
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>164</v>
+        <v>126</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>165</v>
+        <v>127</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>234</v>
+        <v>196</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>233</v>
+        <v>195</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>235</v>
+        <v>197</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>236</v>
+        <v>198</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>237</v>
+        <v>199</v>
       </c>
       <c r="G113" s="2" t="s">
-        <v>238</v>
+        <v>200</v>
       </c>
       <c r="H113" s="3" t="s">
-        <v>246</v>
+        <v>208</v>
       </c>
       <c r="I113" s="3" t="s">
-        <v>239</v>
+        <v>201</v>
       </c>
       <c r="J113" s="6" t="s">
-        <v>248</v>
+        <v>210</v>
       </c>
       <c r="K113" s="6" t="s">
-        <v>249</v>
+        <v>211</v>
       </c>
       <c r="L113" s="6" t="s">
-        <v>247</v>
+        <v>209</v>
       </c>
       <c r="M113" s="6" t="s">
-        <v>250</v>
+        <v>212</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>168</v>
+        <v>130</v>
       </c>
       <c r="B114" t="s">
         <v>46</v>
@@ -4924,7 +4924,7 @@
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>169</v>
+        <v>131</v>
       </c>
       <c r="B115" t="s">
         <v>21</v>
@@ -4965,7 +4965,7 @@
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
       <c r="B116" t="s">
         <v>1</v>
@@ -5006,7 +5006,7 @@
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>171</v>
+        <v>133</v>
       </c>
       <c r="B117" t="s">
         <v>0</v>
@@ -5047,7 +5047,7 @@
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>172</v>
+        <v>134</v>
       </c>
       <c r="B118" t="s">
         <v>47</v>
@@ -5088,7 +5088,7 @@
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>173</v>
+        <v>135</v>
       </c>
       <c r="B119" t="s">
         <v>48</v>
@@ -5129,7 +5129,7 @@
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>174</v>
+        <v>136</v>
       </c>
       <c r="B120" t="s">
         <v>49</v>
@@ -5170,7 +5170,7 @@
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="B121" t="s">
         <v>50</v>
@@ -5208,7 +5208,7 @@
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
       <c r="B122" t="s">
         <v>51</v>
@@ -5249,7 +5249,7 @@
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>177</v>
+        <v>139</v>
       </c>
       <c r="B123" t="s">
         <v>52</v>
@@ -5287,7 +5287,7 @@
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>178</v>
+        <v>140</v>
       </c>
       <c r="B124" t="s">
         <v>53</v>
@@ -5328,7 +5328,7 @@
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>179</v>
+        <v>141</v>
       </c>
       <c r="B125" t="s">
         <v>54</v>
@@ -5366,7 +5366,7 @@
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="B126" t="s">
         <v>55</v>
@@ -5407,7 +5407,7 @@
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>181</v>
+        <v>143</v>
       </c>
       <c r="B127" t="s">
         <v>56</v>
@@ -5445,7 +5445,7 @@
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>182</v>
+        <v>144</v>
       </c>
       <c r="B128" t="s">
         <v>57</v>
@@ -5486,7 +5486,7 @@
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>183</v>
+        <v>145</v>
       </c>
       <c r="B129" t="s">
         <v>58</v>
@@ -5524,7 +5524,7 @@
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>184</v>
+        <v>146</v>
       </c>
       <c r="B130" t="s">
         <v>59</v>
@@ -5565,7 +5565,7 @@
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>185</v>
+        <v>147</v>
       </c>
       <c r="B131" t="s">
         <v>60</v>
@@ -5603,7 +5603,7 @@
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>186</v>
+        <v>148</v>
       </c>
       <c r="B132" t="s">
         <v>13</v>
@@ -5644,7 +5644,7 @@
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="B133" t="s">
         <v>40</v>
@@ -5685,7 +5685,7 @@
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="B134" t="s">
         <v>22</v>
@@ -5726,7 +5726,7 @@
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="B135" t="s">
         <v>61</v>
@@ -5767,7 +5767,7 @@
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>190</v>
+        <v>152</v>
       </c>
       <c r="B136" t="s">
         <v>62</v>
@@ -5808,7 +5808,7 @@
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>191</v>
+        <v>153</v>
       </c>
       <c r="B137" t="s">
         <v>63</v>
@@ -5837,7 +5837,7 @@
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>192</v>
+        <v>154</v>
       </c>
       <c r="B138" t="s">
         <v>44</v>
@@ -5866,7 +5866,7 @@
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>193</v>
+        <v>155</v>
       </c>
       <c r="B139" t="s">
         <v>64</v>
@@ -5907,7 +5907,7 @@
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="B140" t="s">
         <v>65</v>
@@ -5945,7 +5945,7 @@
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="B141" t="s">
         <v>66</v>
@@ -5986,7 +5986,7 @@
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>196</v>
+        <v>158</v>
       </c>
       <c r="B142" t="s">
         <v>67</v>
@@ -6027,7 +6027,7 @@
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>197</v>
+        <v>159</v>
       </c>
       <c r="B143" t="s">
         <v>68</v>
@@ -6068,7 +6068,7 @@
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>198</v>
+        <v>160</v>
       </c>
       <c r="B144" t="s">
         <v>69</v>
@@ -6109,7 +6109,7 @@
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>199</v>
+        <v>161</v>
       </c>
       <c r="B145" t="s">
         <v>70</v>
@@ -6150,7 +6150,7 @@
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="B146" t="s">
         <v>71</v>
@@ -6179,7 +6179,7 @@
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="B147" t="s">
         <v>20</v>
@@ -6208,7 +6208,7 @@
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="B148" t="s">
         <v>72</v>
@@ -6237,7 +6237,7 @@
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
       <c r="B149" t="s">
         <v>73</v>
@@ -6266,7 +6266,7 @@
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>204</v>
+        <v>166</v>
       </c>
       <c r="B150" t="s">
         <v>74</v>
@@ -6307,7 +6307,7 @@
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>205</v>
+        <v>167</v>
       </c>
       <c r="B151" t="s">
         <v>75</v>
@@ -6348,7 +6348,7 @@
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>206</v>
+        <v>168</v>
       </c>
       <c r="B152" t="s">
         <v>76</v>
@@ -6386,7 +6386,7 @@
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>207</v>
+        <v>169</v>
       </c>
       <c r="B153" t="s">
         <v>11</v>
@@ -6427,7 +6427,7 @@
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>208</v>
+        <v>170</v>
       </c>
       <c r="B154" t="s">
         <v>77</v>
@@ -6465,7 +6465,7 @@
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>209</v>
+        <v>171</v>
       </c>
       <c r="B155" t="s">
         <v>64</v>
@@ -6506,7 +6506,7 @@
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>210</v>
+        <v>172</v>
       </c>
       <c r="B156" t="s">
         <v>65</v>
@@ -6544,7 +6544,7 @@
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>211</v>
+        <v>173</v>
       </c>
       <c r="B157" t="s">
         <v>25</v>
@@ -6585,7 +6585,7 @@
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="B158" t="s">
         <v>26</v>
@@ -6626,7 +6626,7 @@
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>213</v>
+        <v>175</v>
       </c>
       <c r="B159" t="s">
         <v>36</v>
@@ -6667,7 +6667,7 @@
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>167</v>
+        <v>129</v>
       </c>
       <c r="B160" t="s">
         <v>45</v>
@@ -6708,7 +6708,7 @@
     </row>
     <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>166</v>
+        <v>128</v>
       </c>
       <c r="B161" t="s">
         <v>23</v>
@@ -6749,7 +6749,7 @@
     </row>
     <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>214</v>
+        <v>176</v>
       </c>
       <c r="B162" t="s">
         <v>78</v>
@@ -6790,7 +6790,7 @@
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>215</v>
+        <v>177</v>
       </c>
       <c r="B163" t="s">
         <v>79</v>
@@ -6831,7 +6831,7 @@
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>216</v>
+        <v>178</v>
       </c>
       <c r="B164" t="s">
         <v>80</v>
@@ -6872,7 +6872,7 @@
     </row>
     <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>217</v>
+        <v>179</v>
       </c>
       <c r="B165" t="s">
         <v>81</v>
@@ -6913,7 +6913,7 @@
     </row>
     <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>218</v>
+        <v>180</v>
       </c>
       <c r="B166" t="s">
         <v>82</v>
@@ -6951,7 +6951,7 @@
     </row>
     <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>219</v>
+        <v>181</v>
       </c>
       <c r="B167" t="s">
         <v>9</v>
@@ -6992,7 +6992,7 @@
     </row>
     <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>220</v>
+        <v>182</v>
       </c>
       <c r="B168" t="s">
         <v>83</v>
@@ -7033,7 +7033,7 @@
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>221</v>
+        <v>183</v>
       </c>
       <c r="B169" t="s">
         <v>84</v>
@@ -7074,7 +7074,7 @@
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>282</v>
+        <v>244</v>
       </c>
       <c r="G170" s="10"/>
       <c r="H170" t="s">
@@ -7086,7 +7086,7 @@
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
       <c r="G171" s="10"/>
       <c r="H171" t="s">
@@ -7098,31 +7098,31 @@
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>284</v>
+        <v>246</v>
       </c>
       <c r="G172" s="10"/>
       <c r="H172" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
       <c r="I172" t="s">
-        <v>240</v>
+        <v>202</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>285</v>
+        <v>247</v>
       </c>
       <c r="G173" s="10"/>
       <c r="H173" t="s">
-        <v>241</v>
+        <v>203</v>
       </c>
       <c r="I173" t="s">
-        <v>241</v>
+        <v>203</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>286</v>
+        <v>248</v>
       </c>
       <c r="G174" s="10"/>
       <c r="H174" t="s">
@@ -7134,47 +7134,47 @@
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>287</v>
+        <v>249</v>
       </c>
       <c r="G175" s="10"/>
       <c r="H175" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
       <c r="I175" t="s">
-        <v>242</v>
+        <v>204</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>288</v>
+        <v>250</v>
       </c>
       <c r="H176" t="s">
-        <v>243</v>
+        <v>205</v>
       </c>
       <c r="I176" t="s">
-        <v>243</v>
+        <v>205</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>289</v>
+        <v>251</v>
       </c>
       <c r="H177" t="s">
-        <v>244</v>
+        <v>206</v>
       </c>
       <c r="I177" t="s">
-        <v>244</v>
+        <v>206</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>290</v>
+        <v>252</v>
       </c>
       <c r="H178" t="s">
-        <v>245</v>
+        <v>207</v>
       </c>
       <c r="I178" t="s">
-        <v>245</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>